<commit_message>
Updated Nucleo board pinout
</commit_message>
<xml_diff>
--- a/Documents/Nucleo to Board coloured pinout.xlsx
+++ b/Documents/Nucleo to Board coloured pinout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\!ENG_PROJECT\engineering-project-v\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\FSSTU04D\STU12\Home\Ddreise6630\!ENG_PROJECT\engineering-project-v\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B939A37A-E496-416C-A542-E8EF1B1ECBC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D787D22-4A5C-4FDB-8C13-C8D2AC64A66D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{1E726284-65D2-40F9-8649-F8952536B159}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Dan's Board</t>
   </si>
@@ -111,6 +111,39 @@
   </si>
   <si>
     <t>RS232_Rx</t>
+  </si>
+  <si>
+    <t>CAN_RX</t>
+  </si>
+  <si>
+    <t>CAN_TX</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>ENCODER_1</t>
+  </si>
+  <si>
+    <t>ENCODER_2</t>
+  </si>
+  <si>
+    <t>Limit_Switch_1</t>
+  </si>
+  <si>
+    <t>Limit_Switch_2</t>
+  </si>
+  <si>
+    <t>DC_1.1</t>
+  </si>
+  <si>
+    <t>DC_1.2</t>
+  </si>
+  <si>
+    <t>DC_2.1</t>
+  </si>
+  <si>
+    <t>DC_2.2</t>
   </si>
 </sst>
 </file>
@@ -156,7 +189,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +247,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +349,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -432,6 +471,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -752,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3299C4E1-746B-4993-871F-28222AED9D27}">
-  <dimension ref="C1:Z29"/>
+  <dimension ref="C1:Z30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y20" sqref="Y20"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -926,7 +976,9 @@
       <c r="O7" s="4">
         <v>3</v>
       </c>
-      <c r="P7" s="13"/>
+      <c r="P7" s="51">
+        <v>3</v>
+      </c>
       <c r="Q7" s="14"/>
       <c r="R7" s="5">
         <v>4</v>
@@ -974,7 +1026,9 @@
       <c r="O8" s="4">
         <v>5</v>
       </c>
-      <c r="P8" s="13"/>
+      <c r="P8" s="16">
+        <v>3</v>
+      </c>
       <c r="Q8" s="19"/>
       <c r="R8" s="5">
         <v>6</v>
@@ -1099,7 +1153,7 @@
         <v>11</v>
       </c>
       <c r="I11" s="13"/>
-      <c r="J11" s="14"/>
+      <c r="J11" s="19"/>
       <c r="K11" s="7">
         <v>12</v>
       </c>
@@ -1140,7 +1194,9 @@
       <c r="H12" s="6">
         <v>13</v>
       </c>
-      <c r="I12" s="13"/>
+      <c r="I12" s="37">
+        <v>2</v>
+      </c>
       <c r="J12" s="14"/>
       <c r="K12" s="7">
         <v>14</v>
@@ -1148,7 +1204,9 @@
       <c r="O12" s="4">
         <v>13</v>
       </c>
-      <c r="P12" s="13"/>
+      <c r="P12" s="50">
+        <v>3</v>
+      </c>
       <c r="Q12" s="14"/>
       <c r="R12" s="5">
         <v>14</v>
@@ -1158,7 +1216,9 @@
         <v>13</v>
       </c>
       <c r="U12" s="13"/>
-      <c r="V12" s="14"/>
+      <c r="V12" s="56">
+        <v>2</v>
+      </c>
       <c r="W12" s="7">
         <v>14</v>
       </c>
@@ -1182,7 +1242,9 @@
       <c r="H13" s="6">
         <v>15</v>
       </c>
-      <c r="I13" s="13"/>
+      <c r="I13" s="59">
+        <v>1</v>
+      </c>
       <c r="J13" s="20">
         <v>1</v>
       </c>
@@ -1192,7 +1254,9 @@
       <c r="O13" s="4">
         <v>15</v>
       </c>
-      <c r="P13" s="13"/>
+      <c r="P13" s="60">
+        <v>2</v>
+      </c>
       <c r="Q13" s="14"/>
       <c r="R13" s="5">
         <v>16</v>
@@ -1218,7 +1282,6 @@
         <v>17</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="E14" s="14"/>
       <c r="F14" s="5">
         <v>18</v>
       </c>
@@ -1250,7 +1313,9 @@
         <v>17</v>
       </c>
       <c r="U14" s="23"/>
-      <c r="V14" s="19"/>
+      <c r="V14" s="56">
+        <v>1</v>
+      </c>
       <c r="W14" s="7">
         <v>18</v>
       </c>
@@ -1324,7 +1389,9 @@
       <c r="H16" s="6">
         <v>21</v>
       </c>
-      <c r="I16" s="23"/>
+      <c r="I16" s="50">
+        <v>3</v>
+      </c>
       <c r="J16" s="14"/>
       <c r="K16" s="7">
         <v>22</v>
@@ -1332,7 +1399,9 @@
       <c r="O16" s="4">
         <v>21</v>
       </c>
-      <c r="P16" s="23"/>
+      <c r="P16" s="21">
+        <v>3</v>
+      </c>
       <c r="Q16" s="14"/>
       <c r="R16" s="5">
         <v>22</v>
@@ -1366,7 +1435,9 @@
       <c r="H17" s="6">
         <v>23</v>
       </c>
-      <c r="I17" s="13"/>
+      <c r="I17" s="60">
+        <v>2</v>
+      </c>
       <c r="J17" s="14"/>
       <c r="K17" s="7">
         <v>24</v>
@@ -1427,7 +1498,9 @@
       <c r="T18" s="6">
         <v>25</v>
       </c>
-      <c r="U18" s="23"/>
+      <c r="U18" s="37">
+        <v>2</v>
+      </c>
       <c r="V18" s="28"/>
       <c r="W18" s="7">
         <v>26</v>
@@ -1526,6 +1599,12 @@
       <c r="W20" s="7">
         <v>30</v>
       </c>
+      <c r="Y20" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="21" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C21" s="4">
@@ -1562,6 +1641,12 @@
       <c r="W21" s="7">
         <v>32</v>
       </c>
+      <c r="Y21" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C22" s="4">
@@ -1602,13 +1687,19 @@
       <c r="W22" s="7">
         <v>34</v>
       </c>
+      <c r="Y22" s="57">
+        <v>1</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="23" spans="3:26" x14ac:dyDescent="0.25">
       <c r="C23" s="4">
         <v>35</v>
       </c>
       <c r="D23" s="13"/>
-      <c r="E23" s="14"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="5">
         <v>36</v>
       </c>
@@ -1644,6 +1735,12 @@
       <c r="W23" s="7">
         <v>36</v>
       </c>
+      <c r="Y23" s="39">
+        <v>2</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="4">
@@ -1669,7 +1766,9 @@
       <c r="P24" s="29">
         <v>1</v>
       </c>
-      <c r="Q24" s="30"/>
+      <c r="Q24" s="30">
+        <v>1</v>
+      </c>
       <c r="R24" s="5">
         <v>38</v>
       </c>
@@ -1683,6 +1782,12 @@
       <c r="V24" s="18"/>
       <c r="W24" s="7">
         <v>38</v>
+      </c>
+      <c r="Y24" s="49">
+        <v>2</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1712,11 +1817,39 @@
       </c>
       <c r="V25" s="9"/>
       <c r="W25" s="10"/>
+      <c r="Y25" s="40">
+        <v>3</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="Y26" s="57">
+        <v>2</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="Y27" s="44">
+        <v>3</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="28" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D28" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="Y28" s="41">
+        <v>3</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="29" spans="3:26" x14ac:dyDescent="0.25">
       <c r="D29" s="36" t="s">
@@ -1725,6 +1858,16 @@
       <c r="E29" s="35" t="s">
         <v>8</v>
       </c>
+      <c r="Y29" s="43">
+        <v>3</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="Y30" s="39"/>
+      <c r="Z30" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1737,6 +1880,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009DB1F523CC530C44BB87B953EC2E8361" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a60fda6cd6ab342f267b2a5945c18740">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6bb3237a-af2d-425e-a269-b1bf50cab29d" xmlns:ns4="3e0af245-5844-467d-8999-70a591b59cc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="772b783578299868aa6ab89439711b81" ns3:_="" ns4:_="">
     <xsd:import namespace="6bb3237a-af2d-425e-a269-b1bf50cab29d"/>
@@ -1959,22 +2117,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{596ABAF4-4311-496C-97A7-162D9A55DD74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6bb3237a-af2d-425e-a269-b1bf50cab29d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3e0af245-5844-467d-8999-70a591b59cc7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{577F57AA-3AF9-43BA-B87F-22E3B872CEF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11716F50-CCF7-4CB8-B555-01E08ED8D140}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1991,29 +2159,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{577F57AA-3AF9-43BA-B87F-22E3B872CEF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{596ABAF4-4311-496C-97A7-162D9A55DD74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6bb3237a-af2d-425e-a269-b1bf50cab29d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3e0af245-5844-467d-8999-70a591b59cc7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated pinout. Some things still need to be changed
</commit_message>
<xml_diff>
--- a/Documents/Nucleo to Board coloured pinout.xlsx
+++ b/Documents/Nucleo to Board coloured pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\!ENG_PROJECT\engineering-project-v\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DA4FD3-9930-49BA-A0D7-0294E01B41E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3996291A-8132-4DE2-B80F-DDD9F5912CED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18510" windowHeight="7170" xr2:uid="{1E726284-65D2-40F9-8649-F8952536B159}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
   <si>
     <t>Dan's Board</t>
   </si>
@@ -147,6 +147,12 @@
   </si>
   <si>
     <t>3V</t>
+  </si>
+  <si>
+    <t>change step2.1 to PA13</t>
+  </si>
+  <si>
+    <t>change STEP2_2 to PA15</t>
   </si>
 </sst>
 </file>
@@ -805,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3299C4E1-746B-4993-871F-28222AED9D27}">
-  <dimension ref="C1:Z30"/>
+  <dimension ref="C1:AC30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -826,7 +832,7 @@
     <col min="25" max="25" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:26" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="3:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="C1" s="58" t="s">
         <v>10</v>
       </c>
@@ -851,7 +857,7 @@
       <c r="V1" s="58"/>
       <c r="W1" s="58"/>
     </row>
-    <row r="2" spans="3:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:29" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="59" t="s">
         <v>11</v>
       </c>
@@ -876,7 +882,7 @@
       <c r="V2" s="60"/>
       <c r="W2" s="60"/>
     </row>
-    <row r="4" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="34" t="s">
         <v>0</v>
       </c>
@@ -884,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
@@ -910,7 +916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C6" s="4">
         <v>1</v>
       </c>
@@ -954,7 +960,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C7" s="4">
         <v>3</v>
       </c>
@@ -1003,8 +1009,11 @@
       <c r="Z7" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AC7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C8" s="4">
         <v>5</v>
       </c>
@@ -1053,8 +1062,11 @@
       <c r="Z8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AC8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C9" s="4">
         <v>7</v>
       </c>
@@ -1100,7 +1112,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C10" s="4">
         <v>9</v>
       </c>
@@ -1142,7 +1154,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C11" s="4">
         <v>11</v>
       </c>
@@ -1184,7 +1196,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C12" s="4">
         <v>13</v>
       </c>
@@ -1229,7 +1241,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C13" s="4">
         <v>15</v>
       </c>
@@ -1278,7 +1290,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C14" s="4">
         <v>17</v>
       </c>
@@ -1327,7 +1339,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C15" s="4">
         <v>19</v>
       </c>
@@ -1375,7 +1387,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C16" s="4">
         <v>21</v>
       </c>
@@ -1885,6 +1897,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009DB1F523CC530C44BB87B953EC2E8361" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a60fda6cd6ab342f267b2a5945c18740">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6bb3237a-af2d-425e-a269-b1bf50cab29d" xmlns:ns4="3e0af245-5844-467d-8999-70a591b59cc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="772b783578299868aa6ab89439711b81" ns3:_="" ns4:_="">
     <xsd:import namespace="6bb3237a-af2d-425e-a269-b1bf50cab29d"/>
@@ -2107,22 +2134,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{596ABAF4-4311-496C-97A7-162D9A55DD74}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="6bb3237a-af2d-425e-a269-b1bf50cab29d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="3e0af245-5844-467d-8999-70a591b59cc7"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{577F57AA-3AF9-43BA-B87F-22E3B872CEF9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11716F50-CCF7-4CB8-B555-01E08ED8D140}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2139,29 +2176,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{577F57AA-3AF9-43BA-B87F-22E3B872CEF9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{596ABAF4-4311-496C-97A7-162D9A55DD74}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="6bb3237a-af2d-425e-a269-b1bf50cab29d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="3e0af245-5844-467d-8999-70a591b59cc7"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>